<commit_message>
Updated ColumnRelationships and DataColumnAttributes.
</commit_message>
<xml_diff>
--- a/VendorRisk_Attributes.xlsx
+++ b/VendorRisk_Attributes.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berutan\Desktop\Projects\ETLDashboard\ETLDashboard\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9E961435-33B2-4119-B202-BF4FAF4ECFC8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Column Attributes" sheetId="1" r:id="rId1"/>
     <sheet name="Column Relationships" sheetId="2" r:id="rId2"/>
     <sheet name="Uniques" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -270,8 +276,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,6 +364,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -404,7 +418,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -436,9 +450,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -470,6 +502,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -645,14 +695,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -708,7 +758,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -758,7 +808,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -814,7 +864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -870,7 +920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -932,14 +982,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R81"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="18" width="10.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -956,13 +1011,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -970,7 +1025,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -1024,12 +1079,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1081,7 +1135,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1089,7 +1143,6 @@
         <v>24</v>
       </c>
       <c r="C6" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1138,7 +1191,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1149,7 +1202,6 @@
         <v>24</v>
       </c>
       <c r="D7" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -1195,7 +1247,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1209,7 +1261,6 @@
         <v>24</v>
       </c>
       <c r="E8" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -1252,7 +1303,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1269,7 +1320,6 @@
         <v>26</v>
       </c>
       <c r="F9" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -1309,7 +1359,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1329,7 +1379,6 @@
         <v>24</v>
       </c>
       <c r="G10" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="H10" s="3" t="s">
@@ -1366,7 +1415,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -1389,7 +1438,6 @@
         <v>25</v>
       </c>
       <c r="H11" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="I11" s="4" t="s">
@@ -1423,7 +1471,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1449,7 +1497,6 @@
         <v>27</v>
       </c>
       <c r="I12" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="J12" s="3" t="s">
@@ -1480,7 +1527,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1509,7 +1556,6 @@
         <v>26</v>
       </c>
       <c r="J13" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="K13" s="2" t="s">
@@ -1537,7 +1583,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1569,7 +1615,6 @@
         <v>24</v>
       </c>
       <c r="K14" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="L14" s="2" t="s">
@@ -1594,7 +1639,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -1629,7 +1674,6 @@
         <v>24</v>
       </c>
       <c r="L15" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="M15" s="3" t="s">
@@ -1651,7 +1695,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
@@ -1689,7 +1733,6 @@
         <v>25</v>
       </c>
       <c r="M16" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="N16" s="4" t="s">
@@ -1708,7 +1751,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -1749,7 +1792,6 @@
         <v>27</v>
       </c>
       <c r="N17" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="O17" s="3" t="s">
@@ -1765,7 +1807,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -1809,7 +1851,6 @@
         <v>26</v>
       </c>
       <c r="O18" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="P18" s="2" t="s">
@@ -1822,7 +1863,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -1869,7 +1910,6 @@
         <v>24</v>
       </c>
       <c r="P19" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="Q19" s="2" t="s">
@@ -1879,7 +1919,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -1929,14 +1969,13 @@
         <v>24</v>
       </c>
       <c r="Q20" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="R20" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -1989,11 +2028,10 @@
         <v>24</v>
       </c>
       <c r="R21" s="5">
-        <f/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
@@ -2001,7 +2039,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>7</v>
@@ -2055,12 +2093,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -2112,7 +2149,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>15</v>
       </c>
@@ -2120,7 +2157,6 @@
         <v>24</v>
       </c>
       <c r="C26" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -2169,7 +2205,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
@@ -2180,7 +2216,6 @@
         <v>24</v>
       </c>
       <c r="D27" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="E27" s="2" t="s">
@@ -2226,7 +2261,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
@@ -2240,7 +2275,6 @@
         <v>24</v>
       </c>
       <c r="E28" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="F28" s="3" t="s">
@@ -2283,7 +2317,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>14</v>
       </c>
@@ -2300,7 +2334,6 @@
         <v>26</v>
       </c>
       <c r="F29" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -2340,7 +2373,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>11</v>
       </c>
@@ -2360,7 +2393,6 @@
         <v>24</v>
       </c>
       <c r="G30" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="H30" s="3" t="s">
@@ -2397,7 +2429,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>1</v>
       </c>
@@ -2420,7 +2452,6 @@
         <v>25</v>
       </c>
       <c r="H31" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="I31" s="4" t="s">
@@ -2454,7 +2485,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>3</v>
       </c>
@@ -2480,7 +2511,6 @@
         <v>27</v>
       </c>
       <c r="I32" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="J32" s="3" t="s">
@@ -2511,7 +2541,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
@@ -2540,7 +2570,6 @@
         <v>26</v>
       </c>
       <c r="J33" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="K33" s="2" t="s">
@@ -2568,7 +2597,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>6</v>
       </c>
@@ -2600,7 +2629,6 @@
         <v>24</v>
       </c>
       <c r="K34" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="L34" s="2" t="s">
@@ -2625,7 +2653,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>12</v>
       </c>
@@ -2660,7 +2688,6 @@
         <v>24</v>
       </c>
       <c r="L35" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="M35" s="3" t="s">
@@ -2682,7 +2709,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>2</v>
       </c>
@@ -2720,7 +2747,6 @@
         <v>25</v>
       </c>
       <c r="M36" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="N36" s="4" t="s">
@@ -2739,7 +2765,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>4</v>
       </c>
@@ -2780,7 +2806,6 @@
         <v>27</v>
       </c>
       <c r="N37" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="O37" s="3" t="s">
@@ -2796,7 +2821,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
@@ -2840,7 +2865,6 @@
         <v>26</v>
       </c>
       <c r="O38" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="P38" s="2" t="s">
@@ -2853,7 +2877,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>10</v>
       </c>
@@ -2900,7 +2924,6 @@
         <v>24</v>
       </c>
       <c r="P39" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="Q39" s="2" t="s">
@@ -2910,7 +2933,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>16</v>
       </c>
@@ -2960,14 +2983,13 @@
         <v>24</v>
       </c>
       <c r="Q40" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="R40" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>17</v>
       </c>
@@ -3020,11 +3042,10 @@
         <v>24</v>
       </c>
       <c r="R41" s="5">
-        <f/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>28</v>
       </c>
@@ -3032,7 +3053,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:18">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
         <v>7</v>
@@ -3086,12 +3107,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:18">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B45" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="C45" s="2" t="s">
@@ -3143,7 +3163,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:18">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>15</v>
       </c>
@@ -3151,7 +3171,6 @@
         <v>24</v>
       </c>
       <c r="C46" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="D46" s="2" t="s">
@@ -3200,7 +3219,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:18">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>5</v>
       </c>
@@ -3211,7 +3230,6 @@
         <v>24</v>
       </c>
       <c r="D47" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="E47" s="2" t="s">
@@ -3257,7 +3275,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:18">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>13</v>
       </c>
@@ -3271,7 +3289,6 @@
         <v>24</v>
       </c>
       <c r="E48" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="F48" s="3" t="s">
@@ -3314,7 +3331,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:18">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>14</v>
       </c>
@@ -3331,7 +3348,6 @@
         <v>26</v>
       </c>
       <c r="F49" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="G49" s="2" t="s">
@@ -3371,7 +3387,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:18">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>11</v>
       </c>
@@ -3391,7 +3407,6 @@
         <v>24</v>
       </c>
       <c r="G50" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="H50" s="3" t="s">
@@ -3428,7 +3443,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:18">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>1</v>
       </c>
@@ -3451,7 +3466,6 @@
         <v>25</v>
       </c>
       <c r="H51" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="I51" s="4" t="s">
@@ -3485,7 +3499,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:18">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>3</v>
       </c>
@@ -3511,7 +3525,6 @@
         <v>27</v>
       </c>
       <c r="I52" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="J52" s="3" t="s">
@@ -3542,7 +3555,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:18">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>8</v>
       </c>
@@ -3571,7 +3584,6 @@
         <v>26</v>
       </c>
       <c r="J53" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="K53" s="2" t="s">
@@ -3599,7 +3611,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:18">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>6</v>
       </c>
@@ -3631,7 +3643,6 @@
         <v>24</v>
       </c>
       <c r="K54" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="L54" s="2" t="s">
@@ -3656,7 +3667,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:18">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>12</v>
       </c>
@@ -3691,7 +3702,6 @@
         <v>24</v>
       </c>
       <c r="L55" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="M55" s="3" t="s">
@@ -3713,7 +3723,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:18">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>2</v>
       </c>
@@ -3751,7 +3761,6 @@
         <v>25</v>
       </c>
       <c r="M56" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="N56" s="4" t="s">
@@ -3770,7 +3779,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:18">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>4</v>
       </c>
@@ -3811,7 +3820,6 @@
         <v>27</v>
       </c>
       <c r="N57" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="O57" s="3" t="s">
@@ -3827,7 +3835,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:18">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>9</v>
       </c>
@@ -3871,7 +3879,6 @@
         <v>26</v>
       </c>
       <c r="O58" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="P58" s="2" t="s">
@@ -3884,7 +3891,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:18">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>10</v>
       </c>
@@ -3931,7 +3938,6 @@
         <v>24</v>
       </c>
       <c r="P59" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="Q59" s="2" t="s">
@@ -3941,7 +3947,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:18">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>16</v>
       </c>
@@ -3991,14 +3997,13 @@
         <v>24</v>
       </c>
       <c r="Q60" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="R60" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:18">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>17</v>
       </c>
@@ -4051,11 +4056,10 @@
         <v>24</v>
       </c>
       <c r="R61" s="5">
-        <f/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>28</v>
       </c>
@@ -4063,7 +4067,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:18">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1" t="s">
         <v>7</v>
@@ -4117,12 +4121,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:18">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B65" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="C65" s="2" t="s">
@@ -4174,7 +4177,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:18">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>15</v>
       </c>
@@ -4182,7 +4185,6 @@
         <v>24</v>
       </c>
       <c r="C66" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="D66" s="2" t="s">
@@ -4231,7 +4233,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:18">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>5</v>
       </c>
@@ -4242,7 +4244,6 @@
         <v>24</v>
       </c>
       <c r="D67" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="E67" s="2" t="s">
@@ -4288,7 +4289,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="68" spans="1:18">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>13</v>
       </c>
@@ -4302,7 +4303,6 @@
         <v>24</v>
       </c>
       <c r="E68" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="F68" s="3" t="s">
@@ -4345,7 +4345,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:18">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>14</v>
       </c>
@@ -4362,7 +4362,6 @@
         <v>26</v>
       </c>
       <c r="F69" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="G69" s="2" t="s">
@@ -4402,7 +4401,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="1:18">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>11</v>
       </c>
@@ -4422,7 +4421,6 @@
         <v>24</v>
       </c>
       <c r="G70" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="H70" s="3" t="s">
@@ -4459,7 +4457,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:18">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>1</v>
       </c>
@@ -4482,7 +4480,6 @@
         <v>25</v>
       </c>
       <c r="H71" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="I71" s="4" t="s">
@@ -4516,7 +4513,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="72" spans="1:18">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>3</v>
       </c>
@@ -4542,7 +4539,6 @@
         <v>27</v>
       </c>
       <c r="I72" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="J72" s="3" t="s">
@@ -4573,7 +4569,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:18">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>8</v>
       </c>
@@ -4602,7 +4598,6 @@
         <v>26</v>
       </c>
       <c r="J73" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="K73" s="2" t="s">
@@ -4630,7 +4625,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="74" spans="1:18">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>6</v>
       </c>
@@ -4662,7 +4657,6 @@
         <v>24</v>
       </c>
       <c r="K74" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="L74" s="2" t="s">
@@ -4687,7 +4681,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="75" spans="1:18">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>12</v>
       </c>
@@ -4722,7 +4716,6 @@
         <v>24</v>
       </c>
       <c r="L75" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="M75" s="3" t="s">
@@ -4744,7 +4737,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="76" spans="1:18">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>2</v>
       </c>
@@ -4782,7 +4775,6 @@
         <v>25</v>
       </c>
       <c r="M76" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="N76" s="4" t="s">
@@ -4801,7 +4793,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="77" spans="1:18">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>4</v>
       </c>
@@ -4842,7 +4834,6 @@
         <v>27</v>
       </c>
       <c r="N77" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="O77" s="3" t="s">
@@ -4858,7 +4849,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="78" spans="1:18">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>9</v>
       </c>
@@ -4902,7 +4893,6 @@
         <v>26</v>
       </c>
       <c r="O78" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="P78" s="2" t="s">
@@ -4915,7 +4905,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:18">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>10</v>
       </c>
@@ -4962,7 +4952,6 @@
         <v>24</v>
       </c>
       <c r="P79" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="Q79" s="2" t="s">
@@ -4972,7 +4961,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="80" spans="1:18">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>16</v>
       </c>
@@ -5022,14 +5011,13 @@
         <v>24</v>
       </c>
       <c r="Q80" s="5">
-        <f/>
         <v>0</v>
       </c>
       <c r="R80" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="81" spans="1:18">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>17</v>
       </c>
@@ -5082,7 +5070,6 @@
         <v>24</v>
       </c>
       <c r="R81" s="5">
-        <f/>
         <v>0</v>
       </c>
     </row>
@@ -5092,14 +5079,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H110"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -5107,7 +5094,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -5133,7 +5120,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -5159,7 +5146,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -5185,7 +5172,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -5211,7 +5198,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -5234,7 +5221,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -5254,7 +5241,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>42</v>
       </c>
@@ -5265,7 +5252,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>48</v>
       </c>
@@ -5273,7 +5260,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>49</v>
       </c>
@@ -5281,7 +5268,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>50</v>
       </c>
@@ -5289,7 +5276,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>51</v>
       </c>
@@ -5297,7 +5284,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>42</v>
       </c>
@@ -5305,72 +5292,72 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -5378,7 +5365,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
@@ -5404,7 +5391,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -5430,7 +5417,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -5456,7 +5443,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -5482,7 +5469,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -5505,7 +5492,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -5525,7 +5512,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>42</v>
       </c>
@@ -5536,7 +5523,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>48</v>
       </c>
@@ -5544,7 +5531,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>49</v>
       </c>
@@ -5552,7 +5539,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>50</v>
       </c>
@@ -5560,7 +5547,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>51</v>
       </c>
@@ -5568,7 +5555,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>42</v>
       </c>
@@ -5576,72 +5563,72 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E46" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E48" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E49" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E50" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E51" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E53" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E54" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>28</v>
       </c>
@@ -5649,7 +5636,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>7</v>
       </c>
@@ -5675,7 +5662,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>33</v>
       </c>
@@ -5701,7 +5688,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>34</v>
       </c>
@@ -5727,7 +5714,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>35</v>
       </c>
@@ -5753,7 +5740,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>36</v>
       </c>
@@ -5776,7 +5763,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>37</v>
       </c>
@@ -5796,7 +5783,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>42</v>
       </c>
@@ -5807,7 +5794,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="4:5">
+    <row r="65" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
         <v>48</v>
       </c>
@@ -5815,7 +5802,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="4:5">
+    <row r="66" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
         <v>49</v>
       </c>
@@ -5823,7 +5810,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="4:5">
+    <row r="67" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
         <v>50</v>
       </c>
@@ -5831,7 +5818,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="4:5">
+    <row r="68" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
         <v>51</v>
       </c>
@@ -5839,7 +5826,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="69" spans="4:5">
+    <row r="69" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
         <v>42</v>
       </c>
@@ -5847,72 +5834,72 @@
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="4:5">
+    <row r="70" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E70" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="71" spans="4:5">
+    <row r="71" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E71" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="4:5">
+    <row r="72" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E72" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="73" spans="4:5">
+    <row r="73" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E73" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="4:5">
+    <row r="74" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E74" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="75" spans="4:5">
+    <row r="75" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E75" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="76" spans="4:5">
+    <row r="76" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E76" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="77" spans="4:5">
+    <row r="77" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E77" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="78" spans="4:5">
+    <row r="78" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E78" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="79" spans="4:5">
+    <row r="79" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E79" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="80" spans="4:5">
+    <row r="80" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E80" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E81" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E82" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>28</v>
       </c>
@@ -5920,7 +5907,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>7</v>
       </c>
@@ -5946,7 +5933,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>33</v>
       </c>
@@ -5972,7 +5959,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>34</v>
       </c>
@@ -5998,7 +5985,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>35</v>
       </c>
@@ -6024,7 +6011,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>36</v>
       </c>
@@ -6047,7 +6034,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>37</v>
       </c>
@@ -6067,7 +6054,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>42</v>
       </c>
@@ -6078,7 +6065,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D93" t="s">
         <v>48</v>
       </c>
@@ -6086,7 +6073,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D94" t="s">
         <v>49</v>
       </c>
@@ -6094,7 +6081,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D95" t="s">
         <v>50</v>
       </c>
@@ -6102,7 +6089,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D96" t="s">
         <v>51</v>
       </c>
@@ -6110,7 +6097,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="97" spans="4:5">
+    <row r="97" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D97" t="s">
         <v>42</v>
       </c>
@@ -6118,67 +6105,67 @@
         <v>62</v>
       </c>
     </row>
-    <row r="98" spans="4:5">
+    <row r="98" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E98" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="99" spans="4:5">
+    <row r="99" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E99" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="100" spans="4:5">
+    <row r="100" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E100" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="101" spans="4:5">
+    <row r="101" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E101" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="102" spans="4:5">
+    <row r="102" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E102" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="103" spans="4:5">
+    <row r="103" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E103" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="104" spans="4:5">
+    <row r="104" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E104" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="105" spans="4:5">
+    <row r="105" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E105" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="106" spans="4:5">
+    <row r="106" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E106" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="107" spans="4:5">
+    <row r="107" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E107" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="108" spans="4:5">
+    <row r="108" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E108" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="109" spans="4:5">
+    <row r="109" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E109" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="110" spans="4:5">
+    <row r="110" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E110" t="s">
         <v>73</v>
       </c>

</xml_diff>